<commit_message>
add df for equipment
</commit_message>
<xml_diff>
--- a/data_templates/Equipment_Master.xlsx
+++ b/data_templates/Equipment_Master.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loictiemani/Desktop/MasterDataGovernance/Untitled/Master-Data-Governance-SAP/data_templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C478C0E-480D-F049-899E-01BEB429F336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -589,8 +595,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,13 +659,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -697,7 +711,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -731,6 +745,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -765,9 +780,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -940,14 +956,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -993,7 +1020,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +1043,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1039,7 +1066,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1062,7 +1089,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1112,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1131,7 +1158,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1154,7 +1181,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1177,7 +1204,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1227,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1223,7 +1250,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1273,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1296,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1319,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1315,7 +1342,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1338,7 +1365,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1361,7 +1388,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1384,7 +1411,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1407,7 +1434,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1430,7 +1457,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1453,7 +1480,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1476,7 +1503,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1499,7 +1526,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1522,7 +1549,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1545,7 +1572,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1595,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1591,7 +1618,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1614,7 +1641,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1637,7 +1664,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1660,7 +1687,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1683,7 +1710,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1706,7 +1733,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1729,7 +1756,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1752,7 +1779,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1775,7 +1802,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1798,7 +1825,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1848,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1844,7 +1871,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1867,7 +1894,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1890,7 +1917,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1913,7 +1940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1936,7 +1963,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1959,7 +1986,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1982,7 +2009,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2005,7 +2032,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2028,7 +2055,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2051,7 +2078,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2074,7 +2101,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2097,7 +2124,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>

</xml_diff>